<commit_message>
Fixed graph title. Added graph image
</commit_message>
<xml_diff>
--- a/datagrump/PA2_partA_graph.xlsx
+++ b/datagrump/PA2_partA_graph.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Stanford\Senior\Spring\cs 244\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\cs244-pa2\datagrump\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -109,6 +109,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Throughput vs.</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 95th percentile delay</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -190,7 +220,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2AF9820D-CEE4-407B-8ABB-3EFF715E39B2}" type="CELLRANGE">
+                    <a:fld id="{77319E7C-3FE2-4FFC-94EA-7C6EE5F26633}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -226,7 +256,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C36F58EB-32B4-481E-B220-5AED2A53E71E}" type="CELLRANGE">
+                    <a:fld id="{F9D3A801-7073-4C3E-9981-3CE372A52DAB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -262,7 +292,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{754289BD-EDDD-4A5B-B2DA-4AF7E0AC6E4A}" type="CELLRANGE">
+                    <a:fld id="{AAFC97EC-A474-4E1E-AAA2-3B2A369F408A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -298,7 +328,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FCD9434E-197D-40A0-8BA7-CAE1B768E3BC}" type="CELLRANGE">
+                    <a:fld id="{B57E2316-186E-4102-9FC6-5CB8D14A0711}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -334,7 +364,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B55DD868-7383-46E1-A252-0095FB624DC1}" type="CELLRANGE">
+                    <a:fld id="{166EFFC5-06E2-4109-9817-6113353425E2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -370,7 +400,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B4E3B244-A058-4618-A3F5-B189297CD3ED}" type="CELLRANGE">
+                    <a:fld id="{77BAB233-9C5C-43E2-88C2-66CD86446ECB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -406,7 +436,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE754581-930A-4606-96D5-F84F20499A43}" type="CELLRANGE">
+                    <a:fld id="{69D6E901-23C5-4BAB-AE64-0468CF2B7060}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -442,7 +472,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B19E20C7-9BA6-4982-B8D1-AB133C171C64}" type="CELLRANGE">
+                    <a:fld id="{AE7F9C1F-DC2A-4C1F-A19A-F0F95EB93589}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -478,7 +508,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C765424C-B772-4281-B7E8-B16387EFB6D7}" type="CELLRANGE">
+                    <a:fld id="{2D5220F7-B5F1-4B98-97E3-60E6DA7C6105}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1859,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>